<commit_message>
Add Student Report Card
</commit_message>
<xml_diff>
--- a/Student_Report_Card.xlsx
+++ b/Student_Report_Card.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>NAME</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>Column10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -387,7 +384,245 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="16">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -412,261 +647,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -687,26 +667,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K22" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K22" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A1:K22"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="STUDENT REPORT CARD" dataDxfId="12"/>
-    <tableColumn id="2" name="Column1" dataDxfId="11"/>
-    <tableColumn id="3" name="Column2" dataDxfId="10"/>
-    <tableColumn id="4" name="Column3" dataDxfId="9"/>
-    <tableColumn id="5" name="Column4" dataDxfId="8"/>
-    <tableColumn id="6" name="Column5" dataDxfId="7"/>
-    <tableColumn id="7" name="Column6" dataDxfId="6"/>
-    <tableColumn id="8" name="Column7" dataDxfId="5">
+    <tableColumn id="1" name="STUDENT REPORT CARD" dataDxfId="10"/>
+    <tableColumn id="2" name="Column1" dataDxfId="9"/>
+    <tableColumn id="3" name="Column2" dataDxfId="8"/>
+    <tableColumn id="4" name="Column3" dataDxfId="7"/>
+    <tableColumn id="5" name="Column4" dataDxfId="6"/>
+    <tableColumn id="6" name="Column5" dataDxfId="5"/>
+    <tableColumn id="7" name="Column6" dataDxfId="4"/>
+    <tableColumn id="8" name="Column7" dataDxfId="3">
       <calculatedColumnFormula>SUM(C2:G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Column8" dataDxfId="4">
+    <tableColumn id="9" name="Column8" dataDxfId="2">
       <calculatedColumnFormula>(H2/500)*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Column9" dataDxfId="3">
+    <tableColumn id="10" name="Column9" dataDxfId="1">
       <calculatedColumnFormula>IF(I2&gt;=40,"PASS","FAIL")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Column10" dataDxfId="2">
+    <tableColumn id="11" name="Column10" dataDxfId="0">
       <calculatedColumnFormula>IF(I2&gt;=85,"A",IF(I2&gt;=70,"B",IF(I2&gt;=55,"C",IF(I2&gt;=40,"D","F"))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -979,9 +959,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,8 +1246,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>42</v>
+      <c r="A8" s="14">
+        <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>15</v>

</xml_diff>